<commit_message>
Agent step completed: Update Excel export functionality to use proper Microsoft Excel format
</commit_message>
<xml_diff>
--- a/vnexpress_articles.xlsx
+++ b/vnexpress_articles.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,13 +28,25 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004F81BD"/>
+        <bgColor rgb="004F81BD"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,10 +67,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,6 +447,11 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="9" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -451,731 +471,731 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>4812573</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/my-bat-dau-kiem-phieu-bau-tong-thong-4812573.html</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Báo Mỹ nói Donald Trump đắc cử tổng thống Mỹ</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>4812723</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/tam-trang-nguoi-my-trong-luc-cho-ket-qua-bau-cu-4812723.html</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>Tâm trạng người Mỹ trong lúc chờ kết quả bầu cử</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>4812787</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/dang-cong-hoa-gianh-da-so-thuong-vien-my-4812787.html</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>Đảng Cộng hòa giành đa số Thượng viện Mỹ</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>4812730</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/barron-trump-lan-dau-di-bo-phieu-4812730.html</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>Barron Trump lần đầu đi bỏ phiếu</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>4812674</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/vui-buon-cua-phe-cong-hoa-dan-chu-khi-ong-trump-dan-truoc-4812674.html</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>Vui, buồn của phe Cộng hòa - Dân chủ khi ông Trump dẫn trước</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>4812752</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/nevada-gap-rac-roi-vi-cu-tri-tre-khong-biet-ky-ten-4812752.html</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>Nevada gặp rắc rối vì cử tri trẻ không biết ký tên</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>4812592</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/nuoc-my-trong-ngay-bau-cu-4812592.html</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>Nước Mỹ trong ngày bầu cử</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>4812571</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/nhung-nguoi-nhap-cu-my-neu-ly-do-bau-cho-ong-trump-4812571.html</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>Những người nhập cư Mỹ nêu lý do bầu cho ông Trump</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>4812603</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/cu-tri-kien-elon-musk-vi-khong-chon-ngau-nhien-nguoi-nhan-mot-trieu-usd-4812603.html</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>Cử tri kiện Elon Musk vì không chọn ngẫu nhiên người nhận một triệu USD</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>4812584</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/cu-tri-ung-ho-ong-trump-ve-kinh-te-ba-harris-ve-quyen-pha-thai-4812584.html</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>Cử tri ủng hộ ông Trump về kinh tế, bà Harris về quyền phá thai</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>4810598</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/giang-co-o-7-bang-chien-truong-dinh-doat-bau-cu-my-4810598.html</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>Ông Trump áp đảo ở các bang chiến trường</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>4811304</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/truyen-thong-my-xuong-ten-nguoi-dac-cu-the-nao-4811304.html</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>Truyền thông Mỹ xướng tên người đắc cử thế nào</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>4810347</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/ly-do-my-kho-cong-bo-nguoi-chien-thang-ngay-dem-bau-cu-4810347.html</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>Lý do Mỹ khó công bố người chiến thắng ngay đêm bầu cử</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>4812306</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/nguoi-my-goc-viet-neu-ly-do-bau-cho-trump-harris-4812306.html</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>Người Mỹ gốc Việt nêu lý do bầu cho Trump, Harris</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>4812574</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/thu-tuong-israel-sa-thai-bo-truong-quoc-phong-4812574.html</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr">
         <is>
           <t>Thủ tướng Israel sa thải Bộ trưởng Quốc phòng</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>4812524</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/nguoi-dan-khap-the-gioi-theo-doi-bau-cu-tong-thong-my-4812524.html</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>Người dân khắp thế giới theo dõi bầu cử tổng thống Mỹ</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>4812566</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/nga-cao-buoc-ukraine-dinh-chiem-nha-may-dien-hat-nhan-o-kursk-4812566.html</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="2" t="inlineStr">
         <is>
           <t>Nga cáo buộc Ukraine định chiếm nhà máy điện hạt nhân ở Kursk</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>4812516</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/noi-stress-cua-cu-tri-my-trong-ky-bau-cu-4812516.html</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="2" t="inlineStr">
         <is>
           <t>Nỗi stress của cử tri Mỹ trong kỳ bầu cử</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>4812442</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/cach-gioi-chuc-my-ngan-phieu-bau-ma-4812442.html</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="2" t="inlineStr">
         <is>
           <t>Cách giới chức Mỹ ngăn 'phiếu bầu ma'</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="2" t="inlineStr">
         <is>
           <t>4812551</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/ly-do-ong-trump-van-duoc-bo-phieu-du-da-bi-ket-toi-4812551.html</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="2" t="inlineStr">
         <is>
           <t>Lý do ông Trump vẫn được bỏ phiếu dù đã bị kết tội</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr">
         <is>
           <t>4812547</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/tiem-kich-an-do-xoay-nhu-la-vang-khi-roi-xuong-dat-4812547.html</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="2" t="inlineStr">
         <is>
           <t>Tiêm kích Ấn Độ 'xoay như lá vàng' khi rơi xuống đất</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>4812478</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/nguoi-an-do-toi-den-tho-cau-nguyen-cho-ba-harris-dac-cu-4812478.html</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>Người Ấn Độ tới đền thờ cầu nguyện cho bà Harris đắc cử</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="2" t="inlineStr">
         <is>
           <t>4812154</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/an-so-tu-cu-tri-tham-lang-trong-bau-cu-my-4812154.html</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="2" t="inlineStr">
         <is>
           <t>Ẩn số từ cử tri thầm lặng trong bầu cử Mỹ</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>4811827</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/may-bo-phieu-bau-tong-thong-my-hoat-dong-nhu-the-nao-4811827.html</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="2" t="inlineStr">
         <is>
           <t>Máy bỏ phiếu bầu tổng thống Mỹ hoạt động như thế nào?</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="2" t="inlineStr">
         <is>
           <t>4812341</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/phat-bieu-khep-lai-chien-dich-tranh-cu-cua-trump-harris-4812341.html</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="2" t="inlineStr">
         <is>
           <t>Phát biểu khép lại chiến dịch tranh cử của Trump - Harris</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="2" t="inlineStr">
         <is>
           <t>4812512</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/thu-tuong-tang-chan-dung-chu-tich-ho-chi-minh-cho-khu-di-tich-o-van-nam-4812512.html</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="2" t="inlineStr">
         <is>
           <t>Thủ tướng tặng chân dung Chủ tịch Hồ Chí Minh cho khu di tích ở Vân Nam</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>4812455</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/cac-diem-bo-phieu-bau-tong-thong-tren-khap-nuoc-my-mo-cua-4812455.html</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="2" t="inlineStr">
         <is>
           <t>Ông Trump cáo buộc 'gian lận tràn lan' ở Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="2" t="inlineStr">
         <is>
           <t>4812468</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/vua-tay-ban-nha-duoc-ca-ngoi-vi-dung-vung-truoc-dam-dong-nem-bun-4812468.html</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" s="2" t="inlineStr">
         <is>
           <t>Vua Tây Ban Nha được ca ngợi vì đứng vững trước đám đông ném bùn</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="2" t="inlineStr">
         <is>
           <t>4812291</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/ong-zelensky-nga-phong-uav-vao-ukraine-nhieu-gap-10-lan-nam-ngoai-4812291.html</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" s="2" t="inlineStr">
         <is>
           <t>Ông Zelensky: Nga phóng UAV vào Ukraine nhiều gấp 10 lần năm ngoái</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="2" t="inlineStr">
         <is>
           <t>4812405</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/ha-ma-ngoi-sao-cua-thai-lan-du-doan-ong-trump-dac-cu-4812405.html</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" s="2" t="inlineStr">
         <is>
           <t>Hà mã 'ngôi sao' của Thái Lan dự đoán ông Trump đắc cử</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="2" t="inlineStr">
         <is>
           <t>4812390</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/ong-trump-chon-thanh-pho-dac-biet-lam-diem-van-dong-cuoi-cung-4812390.html</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="2" t="inlineStr">
         <is>
           <t>Ông Trump chọn 'thành phố đặc biệt' làm điểm vận động cuối cùng</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="2" t="inlineStr">
         <is>
           <t>4812160</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/nhung-gia-dinh-my-bat-dong-quan-diem-vi-bau-cu-tong-thong-4812160.html</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="2" t="inlineStr">
         <is>
           <t>Những gia đình Mỹ bất đồng quan điểm vì bầu cử tổng thống</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="2" t="inlineStr">
         <is>
           <t>4812167</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/uav-lancet-co-the-da-tap-kich-hon-2-500-muc-tieu-o-ukraine-4812167.html</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="2" t="inlineStr">
         <is>
           <t>UAV Lancet có thể đã tập kích hơn 2.500 mục tiêu ở Ukraine</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="2" t="inlineStr">
         <is>
           <t>4812177</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/nhung-hinh-anh-dinh-hinh-mua-bau-cu-tong-thong-my-4812177.html</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="2" t="inlineStr">
         <is>
           <t>Những hình ảnh định hình mùa bầu cử tổng thống Mỹ</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="2" t="inlineStr">
         <is>
           <t>4812264</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/nguoi-dan-chuong-trinh-podcast-noi-tieng-tuyen-bo-ung-ho-ong-trump-4812264.html</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" s="2" t="inlineStr">
         <is>
           <t>Người dẫn chương trình podcast nổi tiếng tuyên bố ủng hộ ông Trump</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="2" t="inlineStr">
         <is>
           <t>4812201</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/ong-trump-noi-ba-harris-nen-dau-voi-mike-tyson-4812201.html</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" s="2" t="inlineStr">
         <is>
           <t>Ông Trump nói bà Harris 'nên đấu với Mike Tyson'</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="2" t="inlineStr">
         <is>
           <t>4811297</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/cach-nguoi-my-bo-phieu-va-kiem-dem-ket-qua-bau-cu-4811297.html</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C38" s="2" t="inlineStr">
         <is>
           <t>Cách người Mỹ bỏ phiếu và kiểm đếm kết quả bầu cử</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="2" t="inlineStr">
         <is>
           <t>4812179</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/ba-harris-go-cua-nha-dan-truoc-gio-bau-cu-4812179.html</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="2" t="inlineStr">
         <is>
           <t>Bà Harris gõ cửa nhà dân trước giờ bầu cử</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="2" t="inlineStr">
         <is>
           <t>4812174</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/israel-tuyen-bo-tap-kich-so-chi-huy-tinh-bao-hezbollah-tai-syria-4812174.html</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="2" t="inlineStr">
         <is>
           <t>Israel tuyên bố tập kích 'sở chỉ huy tình báo Hezbollah' tại Syria</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="2" t="inlineStr">
         <is>
           <t>4812119</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/thu-tuong-pham-minh-chinh-len-duong-toi-trung-quoc-4812119.html</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="2" t="inlineStr">
         <is>
           <t>Thủ tướng Phạm Minh Chính lên đường tới Trung Quốc</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="2" t="inlineStr">
         <is>
           <t>4811734</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/thong-diep-doi-choi-cua-trump-va-harris-khi-khep-lai-chien-dich-4811734.html</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="2" t="inlineStr">
         <is>
           <t>Thông điệp đối chọi của Trump và Harris khi khép lại chiến dịch</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="2" t="inlineStr">
         <is>
           <t>4812161</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/ong-trump-ba-harris-van-dong-gio-chot-truoc-bau-cu-4812161.html</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="2" t="inlineStr">
         <is>
           <t>Ông Trump, bà Harris vận động giờ chót trước bầu cử</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44" s="2" t="inlineStr">
         <is>
           <t>4812132</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" s="2" t="inlineStr">
         <is>
           <t>https://vnexpress.net/tham-phan-pennsylvania-cho-phep-elon-musk-thuong-mot-trieu-usd-cho-cu-tri-4812132.html</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C44" s="2" t="inlineStr">
         <is>
           <t>Thẩm phán Pennsylvania cho phép Elon Musk thưởng một triệu USD cho cử tri</t>
         </is>

</xml_diff>

<commit_message>
Agent step completed: Modify the scraper to accept custom URL and XPath selectors as input parameters
</commit_message>
<xml_diff>
--- a/vnexpress_articles.xlsx
+++ b/vnexpress_articles.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,697 +473,799 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>4812920</t>
+          <t>4812969</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ly-do-ba-harris-that-bai-trong-cuoc-dua-vao-nha-trang-4812920.html</t>
+          <t>https://vnexpress.net/quy-mo-thuong-mai-dien-tu-viet-nam-uoc-dat-22-ty-usd-4812969.html</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Lý do bà Harris thất bại trong cuộc đua vào Nhà Trắng</t>
+          <t>Quy mô thương mại điện tử Việt Nam ước đạt 22 tỷ USD</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>4812836</t>
+          <t>4812762</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nguoi-ung-ho-trump-reo-ho-bat-khoc-an-mung-4812836.html</t>
+          <t>https://vnexpress.net/ong-donald-trump-hua-hen-nhung-gi-voi-kinh-te-my-4812762.html</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Người ủng hộ Trump reo hò, bật khóc ăn mừng</t>
+          <t>Ông Donald Trump hứa hẹn những gì với kinh tế Mỹ?</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>4812870</t>
+          <t>4812976</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/lanh-dao-the-gioi-chuc-mung-ong-trump-4812870.html</t>
+          <t>https://vnexpress.net/tuyen-duong-sat-noi-voi-trung-quoc-du-kien-khoi-cong-vao-2025-4812976.html</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Lãnh đạo thế giới chúc mừng ông Trump</t>
+          <t>Tuyến đường sắt nối với Trung Quốc dự kiến khởi công vào 2025</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>4812802</t>
+          <t>4812911</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nguoi-tre-viet-hao-hung-theo-doi-bau-cu-tong-thong-my-4812802.html</t>
+          <t>https://vnexpress.net/nhan-tron-giam-ve-vung-88-trieu-dong-4812911.html</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Người trẻ Việt hào hứng theo dõi bầu cử tổng thống Mỹ</t>
+          <t>Vàng nhẫn trơn giảm về quanh 88 triệu đồng</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>4812787</t>
+          <t>4812924</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/dang-cong-hoa-gianh-da-so-thuong-vien-my-4812787.html</t>
+          <t>https://vnexpress.net/chung-khoan-tang-15-diem-4812924.html</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Đảng Cộng hòa giành đa số Thượng viện Mỹ</t>
+          <t>Chứng khoán tăng 15 điểm</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>4812603</t>
+          <t>4812646</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/cu-tri-kien-elon-musk-vi-khong-chon-ngau-nhien-nguoi-nhan-mot-trieu-usd-4812603.html</t>
+          <t>https://vnexpress.net/bitcoin-cham-71-500-usd-khi-trump-tam-dan-dau-4812646.html</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Cử tri kiện Elon Musk vì không chọn ngẫu nhiên người nhận một triệu USD</t>
+          <t>Bitcoin lập kỷ lục 75.300 USD</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>4810598</t>
+          <t>4812599</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/giang-co-o-7-bang-chien-truong-dinh-doat-bau-cu-my-4810598.html</t>
+          <t>https://vnexpress.net/nvidia-vuot-apple-de-thanh-cong-ty-gia-tri-nhat-the-gioi-4812599.html</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Ông Trump áp đảo ở các bang chiến trường</t>
+          <t>Nvidia vượt Apple để thành công ty giá trị nhất thế giới</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>4812723</t>
+          <t>4812363</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/tam-trang-nguoi-my-trong-luc-cho-ket-qua-bau-cu-4812723.html</t>
+          <t>https://vnexpress.net/ethiopia-gap-kho-khi-cam-xe-xang-chuyen-sang-oto-dien-4812363.html</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Tâm trạng người Mỹ trong lúc chờ kết quả bầu cử</t>
+          <t>Ethiopia gặp khó khi cấm xe xăng chuyển sang ôtô điện</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>4812730</t>
+          <t>4812502</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/barron-trump-lan-dau-di-bo-phieu-4812730.html</t>
+          <t>https://vnexpress.net/thu-thue-tu-chuyen-nhuong-dat-tang-manh-4812502.html</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Barron Trump lần đầu đi bỏ phiếu</t>
+          <t>Thu thuế chuyển nhượng bất động sản ở TP HCM tăng gấp rưỡi</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>4812674</t>
+          <t>4812977</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/vui-buon-cua-phe-cong-hoa-dan-chu-khi-ong-trump-dan-truoc-4812674.html</t>
+          <t>https://vnexpress.net/mobile-money-co-gan-10-trieu-tai-khoan-sau-3-nam-thi-diem-4812977.html</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Vui, buồn của phe Cộng hòa - Dân chủ khi ông Trump dẫn trước</t>
+          <t>Mobile Money có gần 10 triệu tài khoản sau 3 năm thí điểm</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>4812752</t>
+          <t>4812645</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nevada-gap-rac-roi-vi-cu-tri-tre-khong-biet-ky-ten-4812752.html</t>
+          <t>https://vnexpress.net/kiem-soat-quyen-luc-de-giam-ganh-nang-cho-nguoi-duyet-du-an-4812645.html</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>Nevada gặp rắc rối vì cử tri trẻ không biết ký tên</t>
+          <t>'Kiểm soát quyền lực để giảm gánh nặng cho người duyệt dự án'</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>4812592</t>
+          <t>4812590</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nuoc-my-trong-ngay-bau-cu-4812592.html</t>
+          <t>https://vnexpress.net/gia-vang-chung-khoan-my-cung-tang-trong-ngay-bau-cu-4812590.html</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Nước Mỹ trong ngày bầu cử</t>
+          <t>Giá vàng, chứng khoán Mỹ cùng tăng trong ngày bầu cử</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>4812571</t>
+          <t>4811187</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nhung-nguoi-nhap-cu-my-neu-ly-do-bau-cho-ong-trump-4812571.html</t>
+          <t>https://vnexpress.net/temu-phai-nop-thue-the-nao-o-viet-nam-4811187.html</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Những người nhập cư Mỹ nêu lý do bầu cho ông Trump</t>
+          <t>Temu phải nộp thuế thế nào ở Việt Nam</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>4812584</t>
+          <t>4812563</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/cu-tri-ung-ho-ong-trump-ve-kinh-te-ba-harris-ve-quyen-pha-thai-4812584.html</t>
+          <t>https://vnexpress.net/viet-nam-co-hon-9-trieu-tai-khoan-chung-khoan-4812563.html</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Cử tri ủng hộ ông Trump về kinh tế, bà Harris về quyền phá thai</t>
+          <t>Việt Nam có hơn 9 triệu tài khoản chứng khoán</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>4811304</t>
+          <t>4812805</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/truyen-thong-my-xuong-ten-nguoi-dac-cu-the-nao-4811304.html</t>
+          <t>https://vnexpress.net/nha-may-lego-1-3-ty-usd-chay-thu-nghiem-4812805.html</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>Truyền thông Mỹ xướng tên người đắc cử thế nào</t>
+          <t>Nhà máy Lego 1,3 tỷ USD chạy thử nghiệm</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>4812306</t>
+          <t>4812719</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nguoi-my-goc-viet-neu-ly-do-bau-cho-trump-harris-4812306.html</t>
+          <t>https://vnexpress.net/vinhomes-va-vinfast-la-thuong-hieu-quoc-gia-4812719.html</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Người Mỹ gốc Việt nêu lý do bầu cho Trump, Harris</t>
+          <t>Vinhomes và VinFast là thương hiệu quốc gia</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>4812574</t>
+          <t>4812510</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/thu-tuong-israel-sa-thai-bo-truong-quoc-phong-4812574.html</t>
+          <t>https://vnexpress.net/vib-nhan-ky-luc-ve-tinh-nang-ca-nhan-hoa-thiet-ke-the-tin-dung-4812510.html</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>Thủ tướng Israel sa thải Bộ trưởng Quốc phòng</t>
+          <t>VIB nhận kỷ lục về tính năng cá nhân hóa thiết kế thẻ tín dụng</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>4812524</t>
+          <t>4812450</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nguoi-dan-khap-the-gioi-theo-doi-bau-cu-tong-thong-my-4812524.html</t>
+          <t>https://vnexpress.net/hai-phong-giai-ngan-gan-9-500-ty-von-dau-tu-cong-4812450.html</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>Người dân khắp thế giới theo dõi bầu cử tổng thống Mỹ</t>
+          <t>Hải Phòng giải ngân gần 9.500 tỷ vốn đầu tư công</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>4812566</t>
+          <t>4812537</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nga-cao-buoc-ukraine-dinh-chiem-nha-may-dien-hat-nhan-o-kursk-4812566.html</t>
+          <t>https://vnexpress.net/keo-dai-thoi-gian-thi-diem-cho-nguoi-viet-vao-choi-casino-4812537.html</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Nga cáo buộc Ukraine định chiếm nhà máy điện hạt nhân ở Kursk</t>
+          <t>Kéo dài thời gian thí điểm cho người Việt vào chơi casino</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>4812516</t>
+          <t>4812530</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/noi-stress-cua-cu-tri-my-trong-ky-bau-cu-4812516.html</t>
+          <t>https://vnexpress.net/doanh-nghiep-muon-mua-du-an-cua-ong-dung-lo-voi-bao-lo-4812530.html</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Nỗi stress của cử tri Mỹ trong kỳ bầu cử</t>
+          <t>Doanh nghiệp muốn mua dự án của ông Dũng 'Lò Vôi' báo lỗ</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>4812442</t>
+          <t>4812449</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/cach-gioi-chuc-my-ngan-phieu-bau-ma-4812442.html</t>
+          <t>https://vnexpress.net/chung-khoan-hom-nay-5-11-vn-index-co-phien-ru-ngu-nha-dau-tu-4812449.html</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Cách giới chức Mỹ ngăn 'phiếu bầu ma'</t>
+          <t>Thanh khoản chứng khoán giảm mạnh</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>4810347</t>
+          <t>4812386</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ly-do-my-kho-cong-bo-nguoi-chien-thang-ngay-dem-bau-cu-4810347.html</t>
+          <t>https://vnexpress.net/cong-nhan-boeing-dung-dinh-cong-4812386.html</t>
         </is>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>Lý do Mỹ khó công bố người chiến thắng ngay đêm bầu cử</t>
+          <t>Công nhân Boeing dừng đình công</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>4812551</t>
+          <t>4812352</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ly-do-ong-trump-van-duoc-bo-phieu-du-da-bi-ket-toi-4812551.html</t>
+          <t>https://vnexpress.net/pho-thu-tuong-se-dung-ai-kiem-soat-doanh-thu-tren-san-thuong-mai-dien-tu-4812352.html</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>Lý do ông Trump vẫn được bỏ phiếu dù đã bị kết tội</t>
+          <t>Phó thủ tướng: Sẽ dùng AI kiểm soát doanh thu trên sàn thương mại điện tử</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>4812547</t>
+          <t>4812272</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/tiem-kich-an-do-xoay-nhu-la-vang-khi-roi-xuong-dat-4812547.html</t>
+          <t>https://vnexpress.net/viet-nam-chi-gan-1-2-ty-usd-nhap-khau-gao-4812272.html</t>
         </is>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>Tiêm kích Ấn Độ 'xoay như lá vàng' khi rơi xuống đất</t>
+          <t>Việt Nam chi gần 1,2 tỷ USD nhập khẩu gạo</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>4812478</t>
+          <t>4811603</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nguoi-an-do-toi-den-tho-cau-nguyen-cho-ba-harris-dac-cu-4812478.html</t>
+          <t>https://vnexpress.net/xuat-khau-sang-my-the-nao-khi-trump-hoac-harris-thang-cu-4811603.html</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>Người Ấn Độ tới đền thờ cầu nguyện cho bà Harris đắc cử</t>
+          <t>Xuất khẩu sang Mỹ thế nào khi Trump hoặc Harris thắng cử</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>4812154</t>
+          <t>4811459</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/an-so-tu-cu-tri-tham-lang-trong-bau-cu-my-4812154.html</t>
+          <t>https://vnexpress.net/kich-ban-gia-vang-va-chung-khoan-sau-ky-bau-cu-my-4811459.html</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>Ẩn số từ cử tri thầm lặng trong bầu cử Mỹ</t>
+          <t>Kịch bản giá vàng và chứng khoán sau kỳ bầu cử Mỹ</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>4811827</t>
+          <t>4812506</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/may-bo-phieu-bau-tong-thong-my-hoat-dong-nhu-the-nao-4811827.html</t>
+          <t>https://vnexpress.net/hang-khong-dang-phuc-hoi-4812506.html</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>Máy bỏ phiếu bầu tổng thống Mỹ hoạt động như thế nào?</t>
+          <t>Hàng không đang phục hồi</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>4812341</t>
+          <t>4812302</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/phat-bieu-khep-lai-chien-dich-tranh-cu-cua-trump-harris-4812341.html</t>
+          <t>https://vnexpress.net/nganh-ban-le-my-canh-bao-thue-nhap-khau-cua-trump-4812302.html</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>Phát biểu khép lại chiến dịch tranh cử của Trump - Harris</t>
+          <t>Ngành bán lẻ Mỹ cảnh báo thuế nhập khẩu của Trump</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>4812512</t>
+          <t>4811919</t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/thu-tuong-tang-chan-dung-chu-tich-ho-chi-minh-cho-khu-di-tich-o-van-nam-4812512.html</t>
+          <t>https://vnexpress.net/thiet-bi-dien-mat-troi-trung-quoc-choi-meo-von-chuot-voi-my-4811919.html</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>Thủ tướng tặng chân dung Chủ tịch Hồ Chí Minh cho khu di tích ở Vân Nam</t>
+          <t>Thiết bị điện mặt trời Trung Quốc chơi 'mèo vờn chuột' với Mỹ</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>4812455</t>
+          <t>4812199</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/cac-diem-bo-phieu-bau-tong-thong-tren-khap-nuoc-my-mo-cua-4812455.html</t>
+          <t>https://vnexpress.net/co-phieu-trump-media-tang-vot-truoc-ngay-bau-cu-my-4812199.html</t>
         </is>
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>Ông Trump cáo buộc 'gian lận tràn lan' ở Philadelphia</t>
+          <t>Cổ phiếu Trump Media tăng vọt trước ngày bầu cử Mỹ</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>4812468</t>
+          <t>4811974</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/vua-tay-ban-nha-duoc-ca-ngoi-vi-dung-vung-truoc-dam-dong-nem-bun-4812468.html</t>
+          <t>https://vnexpress.net/ong-trump-khien-dong-von-tram-ty-usd-vao-my-thap-thom-4811974.html</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>Vua Tây Ban Nha được ca ngợi vì đứng vững trước đám đông ném bùn</t>
+          <t>Ông Trump khiến dòng vốn trăm tỷ USD vào Mỹ thấp thỏm</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>4812291</t>
+          <t>4811962</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ong-zelensky-nga-phong-uav-vao-ukraine-nhieu-gap-10-lan-nam-ngoai-4812291.html</t>
+          <t>https://vnexpress.net/gia-ca-phe-quay-dau-giam-4811962.html</t>
         </is>
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>Ông Zelensky: Nga phóng UAV vào Ukraine nhiều gấp 10 lần năm ngoái</t>
+          <t>Giá cà phê quay đầu giảm</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>4812405</t>
+          <t>4812439</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ha-ma-ngoi-sao-cua-thai-lan-du-doan-ong-trump-dac-cu-4812405.html</t>
+          <t>https://vnexpress.net/loat-hoat-dong-ky-niem-sinh-nhat-20-nam-cua-vincom-4812439.html</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>Hà mã 'ngôi sao' của Thái Lan dự đoán ông Trump đắc cử</t>
+          <t>Loạt hoạt động kỷ niệm sinh nhật 20 năm của Vincom</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>4812390</t>
+          <t>4812448</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ong-trump-chon-thanh-pho-dac-biet-lam-diem-van-dong-cuoi-cung-4812390.html</t>
+          <t>https://vnexpress.net/yeu-to-giup-bidv-dat-thuong-hieu-quoc-gia-4812448.html</t>
         </is>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>Ông Trump chọn 'thành phố đặc biệt' làm điểm vận động cuối cùng</t>
+          <t>Yếu tố giúp BIDV đạt thương hiệu quốc gia</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t>4812160</t>
+          <t>4812496</t>
         </is>
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nhung-gia-dinh-my-bat-dong-quan-diem-vi-bau-cu-tong-thong-4812160.html</t>
+          <t>https://vnexpress.net/5-san-pham-cua-mobifone-la-thuong-hieu-quoc-gia-viet-nam-2024-4812496.html</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>Những gia đình Mỹ bất đồng quan điểm vì bầu cử tổng thống</t>
+          <t>5 sản phẩm của MobiFone là Thương hiệu quốc gia Việt Nam 2024</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>4812167</t>
+          <t>4812443</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/uav-lancet-co-the-da-tap-kich-hon-2-500-muc-tieu-o-ukraine-4812167.html</t>
+          <t>https://vnexpress.net/agribank-dat-thuong-hieu-quoc-gia-nho-hoat-dong-hieu-qua-4812443.html</t>
         </is>
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t>UAV Lancet có thể đã tập kích hơn 2.500 mục tiêu ở Ukraine</t>
+          <t>Agribank đạt thương hiệu quốc gia nhờ hoạt động hiệu quả</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>4812177</t>
+          <t>4812327</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nhung-hinh-anh-dinh-hinh-mua-bau-cu-tong-thong-my-4812177.html</t>
+          <t>https://vnexpress.net/chien-luoc-xanh-giup-hdbank-dat-thuong-hieu-quoc-gia-4812327.html</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>Những hình ảnh định hình mùa bầu cử tổng thống Mỹ</t>
+          <t>Chiến lược xanh giúp HDBank đạt thương hiệu quốc gia</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>4812264</t>
+          <t>4812100</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nguoi-dan-chuong-trinh-podcast-noi-tieng-tuyen-bo-ung-ho-ong-trump-4812264.html</t>
+          <t>https://vnexpress.net/de-xuat-giam-tiep-thue-moi-truong-voi-xang-dau-het-nam-2025-4812100.html</t>
         </is>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>Người dẫn chương trình podcast nổi tiếng tuyên bố ủng hộ ông Trump</t>
+          <t>Đề xuất giảm tiếp thuế môi trường với xăng dầu hết năm 2025</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>4812201</t>
+          <t>4812088</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ong-trump-noi-ba-harris-nen-dau-voi-mike-tyson-4812201.html</t>
+          <t>https://vnexpress.net/evn-de-xuat-thi-diem-gia-dien-hai-thanh-phan-4812088.html</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>Ông Trump nói bà Harris 'nên đấu với Mike Tyson'</t>
+          <t>EVN đề xuất thí điểm giá điện hai thành phần</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>4811297</t>
+          <t>4811845</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/cach-nguoi-my-bo-phieu-va-kiem-dem-ket-qua-bau-cu-4811297.html</t>
+          <t>https://vnexpress.net/opec-lai-hoan-ke-hoach-tang-bom-dau-4811845.html</t>
         </is>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>Cách người Mỹ bỏ phiếu và kiểm đếm kết quả bầu cử</t>
+          <t>OPEC+ lại hoãn kế hoạch tăng bơm dầu</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>4812179</t>
+          <t>4812022</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ba-harris-go-cua-nha-dan-truoc-gio-bau-cu-4812179.html</t>
+          <t>https://vnexpress.net/doanh-nghiep-tu-nhan-can-co-che-chu-khong-phai-tien-4812022.html</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>Bà Harris gõ cửa nhà dân trước giờ bầu cử</t>
+          <t>'Doanh nghiệp tư nhân cần cơ chế chứ không phải tiền'</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t>4812044</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/chung-khoan-do-lua-vi-co-phieu-ngan-hang-4812044.html</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="inlineStr">
+        <is>
+          <t>Chứng khoán đỏ lửa vì cổ phiếu ngân hàng</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>4811999</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/vang-mieng-giam-nua-trieu-dong-4811999.html</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="inlineStr">
+        <is>
+          <t>Giá vàng miếng giảm, USD lên kịch trần</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>4811981</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/ty-phu-thai-nhan-hon-12-000-ty-dong-co-tuc-sau-7-nam-thau-tom-sabeco-4811981.html</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="inlineStr">
+        <is>
+          <t>Tỷ phú Thái nhận hơn 12.000 tỷ đồng cổ tức sau 7 năm thâu tóm Sabeco</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>4811774</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/nganh-dien-gio-my-lo-trump-tai-dac-cu-4811774.html</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="inlineStr">
+        <is>
+          <t>Ngành điện gió Mỹ lo Trump tái đắc cử</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>4811849</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/lang-phi-hang-tram-nghin-ty-dong-khi-du-an-dau-tu-roi-dap-chieu-4811849.html</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="inlineStr">
+        <is>
+          <t>Lãng phí hàng trăm nghìn tỷ đồng khi dự án đầu tư rồi 'đắp chiếu'</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>4811828</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>https://vnexpress.net/mot-doanh-nghiep-may-lon-khong-co-don-hang-suot-18-thang-4811828.html</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="inlineStr">
+        <is>
+          <t>Một doanh nghiệp may lớn không có đơn hàng suốt 18 tháng</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Agent step completed: Add command-line arguments for custom output filenames
</commit_message>
<xml_diff>
--- a/vnexpress_articles.xlsx
+++ b/vnexpress_articles.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,799 +473,697 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>4812969</t>
+          <t>4813022</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/quy-mo-thuong-mai-dien-tu-viet-nam-uoc-dat-22-ty-usd-4812969.html</t>
+          <t>https://vnexpress.net/nga-hoai-nghi-kha-nang-ong-trump-giai-quyet-xung-dot-ukraine-4813022.html</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Quy mô thương mại điện tử Việt Nam ước đạt 22 tỷ USD</t>
+          <t>Nga hoài nghi khả năng ông Trump giải quyết xung đột Ukraine</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>4812762</t>
+          <t>4812992</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ong-donald-trump-hua-hen-nhung-gi-voi-kinh-te-my-4812762.html</t>
+          <t>https://vnexpress.net/chu-tich-nuoc-luong-cuong-sap-du-apec-tai-peru-4812992.html</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Ông Donald Trump hứa hẹn những gì với kinh tế Mỹ?</t>
+          <t>Chủ tịch nước Lương Cường sắp dự APEC tại Peru</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>4812976</t>
+          <t>4812836</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/tuyen-duong-sat-noi-voi-trung-quoc-du-kien-khoi-cong-vao-2025-4812976.html</t>
+          <t>https://vnexpress.net/nguoi-ung-ho-trump-reo-ho-bat-khoc-an-mung-4812836.html</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Tuyến đường sắt nối với Trung Quốc dự kiến khởi công vào 2025</t>
+          <t>Người ủng hộ Trump reo hò, bật khóc ăn mừng</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>4812911</t>
+          <t>4812870</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nhan-tron-giam-ve-vung-88-trieu-dong-4812911.html</t>
+          <t>https://vnexpress.net/lanh-dao-the-gioi-chuc-mung-ong-trump-4812870.html</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Vàng nhẫn trơn giảm về quanh 88 triệu đồng</t>
+          <t>Lãnh đạo thế giới chúc mừng ông Trump</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>4812924</t>
+          <t>4812802</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/chung-khoan-tang-15-diem-4812924.html</t>
+          <t>https://vnexpress.net/nguoi-tre-viet-hao-hung-theo-doi-bau-cu-tong-thong-my-4812802.html</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Chứng khoán tăng 15 điểm</t>
+          <t>Người trẻ Việt hào hứng theo dõi bầu cử tổng thống Mỹ</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>4812646</t>
+          <t>4812787</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/bitcoin-cham-71-500-usd-khi-trump-tam-dan-dau-4812646.html</t>
+          <t>https://vnexpress.net/dang-cong-hoa-gianh-da-so-thuong-vien-my-4812787.html</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Bitcoin lập kỷ lục 75.300 USD</t>
+          <t>Đảng Cộng hòa giành đa số Thượng viện Mỹ</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>4812599</t>
+          <t>4812603</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nvidia-vuot-apple-de-thanh-cong-ty-gia-tri-nhat-the-gioi-4812599.html</t>
+          <t>https://vnexpress.net/cu-tri-kien-elon-musk-vi-khong-chon-ngau-nhien-nguoi-nhan-mot-trieu-usd-4812603.html</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Nvidia vượt Apple để thành công ty giá trị nhất thế giới</t>
+          <t>Cử tri kiện Elon Musk vì không chọn ngẫu nhiên người nhận một triệu USD</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>4812363</t>
+          <t>4810598</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ethiopia-gap-kho-khi-cam-xe-xang-chuyen-sang-oto-dien-4812363.html</t>
+          <t>https://vnexpress.net/giang-co-o-7-bang-chien-truong-dinh-doat-bau-cu-my-4810598.html</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Ethiopia gặp khó khi cấm xe xăng chuyển sang ôtô điện</t>
+          <t>Ông Trump áp đảo ở các bang chiến trường</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>4812502</t>
+          <t>4812723</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/thu-thue-tu-chuyen-nhuong-dat-tang-manh-4812502.html</t>
+          <t>https://vnexpress.net/tam-trang-nguoi-my-trong-luc-cho-ket-qua-bau-cu-4812723.html</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Thu thuế chuyển nhượng bất động sản ở TP HCM tăng gấp rưỡi</t>
+          <t>Tâm trạng người Mỹ trong lúc chờ kết quả bầu cử</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>4812977</t>
+          <t>4812730</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/mobile-money-co-gan-10-trieu-tai-khoan-sau-3-nam-thi-diem-4812977.html</t>
+          <t>https://vnexpress.net/barron-trump-lan-dau-di-bo-phieu-4812730.html</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Mobile Money có gần 10 triệu tài khoản sau 3 năm thí điểm</t>
+          <t>Barron Trump lần đầu đi bỏ phiếu</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>4812645</t>
+          <t>4812674</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/kiem-soat-quyen-luc-de-giam-ganh-nang-cho-nguoi-duyet-du-an-4812645.html</t>
+          <t>https://vnexpress.net/vui-buon-cua-phe-cong-hoa-dan-chu-khi-ong-trump-dan-truoc-4812674.html</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>'Kiểm soát quyền lực để giảm gánh nặng cho người duyệt dự án'</t>
+          <t>Vui, buồn của phe Cộng hòa - Dân chủ khi ông Trump dẫn trước</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>4812590</t>
+          <t>4812752</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/gia-vang-chung-khoan-my-cung-tang-trong-ngay-bau-cu-4812590.html</t>
+          <t>https://vnexpress.net/nevada-gap-rac-roi-vi-cu-tri-tre-khong-biet-ky-ten-4812752.html</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Giá vàng, chứng khoán Mỹ cùng tăng trong ngày bầu cử</t>
+          <t>Nevada gặp rắc rối vì cử tri trẻ không biết ký tên</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>4811187</t>
+          <t>4812592</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/temu-phai-nop-thue-the-nao-o-viet-nam-4811187.html</t>
+          <t>https://vnexpress.net/nuoc-my-trong-ngay-bau-cu-4812592.html</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Temu phải nộp thuế thế nào ở Việt Nam</t>
+          <t>Nước Mỹ trong ngày bầu cử</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>4812563</t>
+          <t>4812571</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/viet-nam-co-hon-9-trieu-tai-khoan-chung-khoan-4812563.html</t>
+          <t>https://vnexpress.net/nhung-nguoi-nhap-cu-my-neu-ly-do-bau-cho-ong-trump-4812571.html</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Việt Nam có hơn 9 triệu tài khoản chứng khoán</t>
+          <t>Những người nhập cư Mỹ nêu lý do bầu cho ông Trump</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>4812805</t>
+          <t>4812584</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nha-may-lego-1-3-ty-usd-chay-thu-nghiem-4812805.html</t>
+          <t>https://vnexpress.net/cu-tri-ung-ho-ong-trump-ve-kinh-te-ba-harris-ve-quyen-pha-thai-4812584.html</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>Nhà máy Lego 1,3 tỷ USD chạy thử nghiệm</t>
+          <t>Cử tri ủng hộ ông Trump về kinh tế, bà Harris về quyền phá thai</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>4812719</t>
+          <t>4811304</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/vinhomes-va-vinfast-la-thuong-hieu-quoc-gia-4812719.html</t>
+          <t>https://vnexpress.net/truyen-thong-my-xuong-ten-nguoi-dac-cu-the-nao-4811304.html</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Vinhomes và VinFast là thương hiệu quốc gia</t>
+          <t>Truyền thông Mỹ xướng tên người đắc cử thế nào</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>4812510</t>
+          <t>4812306</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/vib-nhan-ky-luc-ve-tinh-nang-ca-nhan-hoa-thiet-ke-the-tin-dung-4812510.html</t>
+          <t>https://vnexpress.net/nguoi-my-goc-viet-neu-ly-do-bau-cho-trump-harris-4812306.html</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>VIB nhận kỷ lục về tính năng cá nhân hóa thiết kế thẻ tín dụng</t>
+          <t>Người Mỹ gốc Việt nêu lý do bầu cho Trump, Harris</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>4812450</t>
+          <t>4812574</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hai-phong-giai-ngan-gan-9-500-ty-von-dau-tu-cong-4812450.html</t>
+          <t>https://vnexpress.net/thu-tuong-israel-sa-thai-bo-truong-quoc-phong-4812574.html</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>Hải Phòng giải ngân gần 9.500 tỷ vốn đầu tư công</t>
+          <t>Thủ tướng Israel sa thải Bộ trưởng Quốc phòng</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>4812537</t>
+          <t>4812524</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/keo-dai-thoi-gian-thi-diem-cho-nguoi-viet-vao-choi-casino-4812537.html</t>
+          <t>https://vnexpress.net/nguoi-dan-khap-the-gioi-theo-doi-bau-cu-tong-thong-my-4812524.html</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Kéo dài thời gian thí điểm cho người Việt vào chơi casino</t>
+          <t>Người dân khắp thế giới theo dõi bầu cử tổng thống Mỹ</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>4812530</t>
+          <t>4812566</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/doanh-nghiep-muon-mua-du-an-cua-ong-dung-lo-voi-bao-lo-4812530.html</t>
+          <t>https://vnexpress.net/nga-cao-buoc-ukraine-dinh-chiem-nha-may-dien-hat-nhan-o-kursk-4812566.html</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Doanh nghiệp muốn mua dự án của ông Dũng 'Lò Vôi' báo lỗ</t>
+          <t>Nga cáo buộc Ukraine định chiếm nhà máy điện hạt nhân ở Kursk</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>4812449</t>
+          <t>4812516</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/chung-khoan-hom-nay-5-11-vn-index-co-phien-ru-ngu-nha-dau-tu-4812449.html</t>
+          <t>https://vnexpress.net/noi-stress-cua-cu-tri-my-trong-ky-bau-cu-4812516.html</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Thanh khoản chứng khoán giảm mạnh</t>
+          <t>Nỗi stress của cử tri Mỹ trong kỳ bầu cử</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>4812386</t>
+          <t>4812442</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/cong-nhan-boeing-dung-dinh-cong-4812386.html</t>
+          <t>https://vnexpress.net/cach-gioi-chuc-my-ngan-phieu-bau-ma-4812442.html</t>
         </is>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>Công nhân Boeing dừng đình công</t>
+          <t>Cách giới chức Mỹ ngăn 'phiếu bầu ma'</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>4812352</t>
+          <t>4810347</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/pho-thu-tuong-se-dung-ai-kiem-soat-doanh-thu-tren-san-thuong-mai-dien-tu-4812352.html</t>
+          <t>https://vnexpress.net/ly-do-my-kho-cong-bo-nguoi-chien-thang-ngay-dem-bau-cu-4810347.html</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>Phó thủ tướng: Sẽ dùng AI kiểm soát doanh thu trên sàn thương mại điện tử</t>
+          <t>Lý do Mỹ khó công bố người chiến thắng ngay đêm bầu cử</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>4812272</t>
+          <t>4812551</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/viet-nam-chi-gan-1-2-ty-usd-nhap-khau-gao-4812272.html</t>
+          <t>https://vnexpress.net/ly-do-ong-trump-van-duoc-bo-phieu-du-da-bi-ket-toi-4812551.html</t>
         </is>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>Việt Nam chi gần 1,2 tỷ USD nhập khẩu gạo</t>
+          <t>Lý do ông Trump vẫn được bỏ phiếu dù đã bị kết tội</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>4811603</t>
+          <t>4812547</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/xuat-khau-sang-my-the-nao-khi-trump-hoac-harris-thang-cu-4811603.html</t>
+          <t>https://vnexpress.net/tiem-kich-an-do-xoay-nhu-la-vang-khi-roi-xuong-dat-4812547.html</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>Xuất khẩu sang Mỹ thế nào khi Trump hoặc Harris thắng cử</t>
+          <t>Tiêm kích Ấn Độ 'xoay như lá vàng' khi rơi xuống đất</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>4811459</t>
+          <t>4812478</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/kich-ban-gia-vang-va-chung-khoan-sau-ky-bau-cu-my-4811459.html</t>
+          <t>https://vnexpress.net/nguoi-an-do-toi-den-tho-cau-nguyen-cho-ba-harris-dac-cu-4812478.html</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>Kịch bản giá vàng và chứng khoán sau kỳ bầu cử Mỹ</t>
+          <t>Người Ấn Độ tới đền thờ cầu nguyện cho bà Harris đắc cử</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>4812506</t>
+          <t>4812154</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hang-khong-dang-phuc-hoi-4812506.html</t>
+          <t>https://vnexpress.net/an-so-tu-cu-tri-tham-lang-trong-bau-cu-my-4812154.html</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>Hàng không đang phục hồi</t>
+          <t>Ẩn số từ cử tri thầm lặng trong bầu cử Mỹ</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>4812302</t>
+          <t>4811827</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/nganh-ban-le-my-canh-bao-thue-nhap-khau-cua-trump-4812302.html</t>
+          <t>https://vnexpress.net/may-bo-phieu-bau-tong-thong-my-hoat-dong-nhu-the-nao-4811827.html</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>Ngành bán lẻ Mỹ cảnh báo thuế nhập khẩu của Trump</t>
+          <t>Máy bỏ phiếu bầu tổng thống Mỹ hoạt động như thế nào?</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>4811919</t>
+          <t>4812341</t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/thiet-bi-dien-mat-troi-trung-quoc-choi-meo-von-chuot-voi-my-4811919.html</t>
+          <t>https://vnexpress.net/phat-bieu-khep-lai-chien-dich-tranh-cu-cua-trump-harris-4812341.html</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>Thiết bị điện mặt trời Trung Quốc chơi 'mèo vờn chuột' với Mỹ</t>
+          <t>Phát biểu khép lại chiến dịch tranh cử của Trump - Harris</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>4812199</t>
+          <t>4812512</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/co-phieu-trump-media-tang-vot-truoc-ngay-bau-cu-my-4812199.html</t>
+          <t>https://vnexpress.net/thu-tuong-tang-chan-dung-chu-tich-ho-chi-minh-cho-khu-di-tich-o-van-nam-4812512.html</t>
         </is>
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>Cổ phiếu Trump Media tăng vọt trước ngày bầu cử Mỹ</t>
+          <t>Thủ tướng tặng chân dung Chủ tịch Hồ Chí Minh cho khu di tích ở Vân Nam</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>4811974</t>
+          <t>4812455</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ong-trump-khien-dong-von-tram-ty-usd-vao-my-thap-thom-4811974.html</t>
+          <t>https://vnexpress.net/cac-diem-bo-phieu-bau-tong-thong-tren-khap-nuoc-my-mo-cua-4812455.html</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>Ông Trump khiến dòng vốn trăm tỷ USD vào Mỹ thấp thỏm</t>
+          <t>Ông Trump cáo buộc 'gian lận tràn lan' ở Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>4811962</t>
+          <t>4812468</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/gia-ca-phe-quay-dau-giam-4811962.html</t>
+          <t>https://vnexpress.net/vua-tay-ban-nha-duoc-ca-ngoi-vi-dung-vung-truoc-dam-dong-nem-bun-4812468.html</t>
         </is>
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>Giá cà phê quay đầu giảm</t>
+          <t>Vua Tây Ban Nha được ca ngợi vì đứng vững trước đám đông ném bùn</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>4812439</t>
+          <t>4812291</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/loat-hoat-dong-ky-niem-sinh-nhat-20-nam-cua-vincom-4812439.html</t>
+          <t>https://vnexpress.net/ong-zelensky-nga-phong-uav-vao-ukraine-nhieu-gap-10-lan-nam-ngoai-4812291.html</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>Loạt hoạt động kỷ niệm sinh nhật 20 năm của Vincom</t>
+          <t>Ông Zelensky: Nga phóng UAV vào Ukraine nhiều gấp 10 lần năm ngoái</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>4812448</t>
+          <t>4812405</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/yeu-to-giup-bidv-dat-thuong-hieu-quoc-gia-4812448.html</t>
+          <t>https://vnexpress.net/ha-ma-ngoi-sao-cua-thai-lan-du-doan-ong-trump-dac-cu-4812405.html</t>
         </is>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>Yếu tố giúp BIDV đạt thương hiệu quốc gia</t>
+          <t>Hà mã 'ngôi sao' của Thái Lan dự đoán ông Trump đắc cử</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t>4812496</t>
+          <t>4812390</t>
         </is>
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/5-san-pham-cua-mobifone-la-thuong-hieu-quoc-gia-viet-nam-2024-4812496.html</t>
+          <t>https://vnexpress.net/ong-trump-chon-thanh-pho-dac-biet-lam-diem-van-dong-cuoi-cung-4812390.html</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>5 sản phẩm của MobiFone là Thương hiệu quốc gia Việt Nam 2024</t>
+          <t>Ông Trump chọn 'thành phố đặc biệt' làm điểm vận động cuối cùng</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>4812443</t>
+          <t>4812160</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/agribank-dat-thuong-hieu-quoc-gia-nho-hoat-dong-hieu-qua-4812443.html</t>
+          <t>https://vnexpress.net/nhung-gia-dinh-my-bat-dong-quan-diem-vi-bau-cu-tong-thong-4812160.html</t>
         </is>
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t>Agribank đạt thương hiệu quốc gia nhờ hoạt động hiệu quả</t>
+          <t>Những gia đình Mỹ bất đồng quan điểm vì bầu cử tổng thống</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>4812327</t>
+          <t>4812167</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/chien-luoc-xanh-giup-hdbank-dat-thuong-hieu-quoc-gia-4812327.html</t>
+          <t>https://vnexpress.net/uav-lancet-co-the-da-tap-kich-hon-2-500-muc-tieu-o-ukraine-4812167.html</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>Chiến lược xanh giúp HDBank đạt thương hiệu quốc gia</t>
+          <t>UAV Lancet có thể đã tập kích hơn 2.500 mục tiêu ở Ukraine</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>4812100</t>
+          <t>4812177</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/de-xuat-giam-tiep-thue-moi-truong-voi-xang-dau-het-nam-2025-4812100.html</t>
+          <t>https://vnexpress.net/nhung-hinh-anh-dinh-hinh-mua-bau-cu-tong-thong-my-4812177.html</t>
         </is>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>Đề xuất giảm tiếp thuế môi trường với xăng dầu hết năm 2025</t>
+          <t>Những hình ảnh định hình mùa bầu cử tổng thống Mỹ</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>4812088</t>
+          <t>4812264</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/evn-de-xuat-thi-diem-gia-dien-hai-thanh-phan-4812088.html</t>
+          <t>https://vnexpress.net/nguoi-dan-chuong-trinh-podcast-noi-tieng-tuyen-bo-ung-ho-ong-trump-4812264.html</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>EVN đề xuất thí điểm giá điện hai thành phần</t>
+          <t>Người dẫn chương trình podcast nổi tiếng tuyên bố ủng hộ ông Trump</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>4811845</t>
+          <t>4812201</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/opec-lai-hoan-ke-hoach-tang-bom-dau-4811845.html</t>
+          <t>https://vnexpress.net/ong-trump-noi-ba-harris-nen-dau-voi-mike-tyson-4812201.html</t>
         </is>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>OPEC+ lại hoãn kế hoạch tăng bơm dầu</t>
+          <t>Ông Trump nói bà Harris 'nên đấu với Mike Tyson'</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>4812022</t>
+          <t>4811297</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/doanh-nghiep-tu-nhan-can-co-che-chu-khong-phai-tien-4812022.html</t>
+          <t>https://vnexpress.net/cach-nguoi-my-bo-phieu-va-kiem-dem-ket-qua-bau-cu-4811297.html</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>'Doanh nghiệp tư nhân cần cơ chế chứ không phải tiền'</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="2" t="inlineStr">
-        <is>
-          <t>4812044</t>
-        </is>
-      </c>
-      <c r="B43" s="2" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/chung-khoan-do-lua-vi-co-phieu-ngan-hang-4812044.html</t>
-        </is>
-      </c>
-      <c r="C43" s="2" t="inlineStr">
-        <is>
-          <t>Chứng khoán đỏ lửa vì cổ phiếu ngân hàng</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="2" t="inlineStr">
-        <is>
-          <t>4811999</t>
-        </is>
-      </c>
-      <c r="B44" s="2" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/vang-mieng-giam-nua-trieu-dong-4811999.html</t>
-        </is>
-      </c>
-      <c r="C44" s="2" t="inlineStr">
-        <is>
-          <t>Giá vàng miếng giảm, USD lên kịch trần</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="2" t="inlineStr">
-        <is>
-          <t>4811981</t>
-        </is>
-      </c>
-      <c r="B45" s="2" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/ty-phu-thai-nhan-hon-12-000-ty-dong-co-tuc-sau-7-nam-thau-tom-sabeco-4811981.html</t>
-        </is>
-      </c>
-      <c r="C45" s="2" t="inlineStr">
-        <is>
-          <t>Tỷ phú Thái nhận hơn 12.000 tỷ đồng cổ tức sau 7 năm thâu tóm Sabeco</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="2" t="inlineStr">
-        <is>
-          <t>4811774</t>
-        </is>
-      </c>
-      <c r="B46" s="2" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/nganh-dien-gio-my-lo-trump-tai-dac-cu-4811774.html</t>
-        </is>
-      </c>
-      <c r="C46" s="2" t="inlineStr">
-        <is>
-          <t>Ngành điện gió Mỹ lo Trump tái đắc cử</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="2" t="inlineStr">
-        <is>
-          <t>4811849</t>
-        </is>
-      </c>
-      <c r="B47" s="2" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/lang-phi-hang-tram-nghin-ty-dong-khi-du-an-dau-tu-roi-dap-chieu-4811849.html</t>
-        </is>
-      </c>
-      <c r="C47" s="2" t="inlineStr">
-        <is>
-          <t>Lãng phí hàng trăm nghìn tỷ đồng khi dự án đầu tư rồi 'đắp chiếu'</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="2" t="inlineStr">
-        <is>
-          <t>4811828</t>
-        </is>
-      </c>
-      <c r="B48" s="2" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/mot-doanh-nghiep-may-lon-khong-co-don-hang-suot-18-thang-4811828.html</t>
-        </is>
-      </c>
-      <c r="C48" s="2" t="inlineStr">
-        <is>
-          <t>Một doanh nghiệp may lớn không có đơn hàng suốt 18 tháng</t>
+          <t>Cách người Mỹ bỏ phiếu và kiểm đếm kết quả bầu cử</t>
         </is>
       </c>
     </row>

</xml_diff>